<commit_message>
Updated noun list, deleted some git files
</commit_message>
<xml_diff>
--- a/fst/dict_sgx.xlsx
+++ b/fst/dict_sgx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d59e73f3ee902bc/Desktop/repos/sguuxs_splicer/fst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBB5815C-3988-47FC-9C22-1722F92138BD}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DD866BF-63A4-4FDD-BFDF-64B9B761C821}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
+    <workbookView xWindow="4992" yWindow="504" windowWidth="17280" windowHeight="10560" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>Entry ID</t>
   </si>
@@ -92,7 +92,136 @@
     <t>łguułgu</t>
   </si>
   <si>
-    <t>child/young one</t>
+    <t>nts'iidz</t>
+  </si>
+  <si>
+    <t>niya'ay</t>
+  </si>
+  <si>
+    <t>nigwaat</t>
+  </si>
+  <si>
+    <t>łgutx̱a'oo</t>
+  </si>
+  <si>
+    <t>waky</t>
+  </si>
+  <si>
+    <t>insiipnsk</t>
+  </si>
+  <si>
+    <t>kw'ida'ts</t>
+  </si>
+  <si>
+    <t>łimkt'ii</t>
+  </si>
+  <si>
+    <t>daala</t>
+  </si>
+  <si>
+    <t>waa</t>
+  </si>
+  <si>
+    <t>waalp</t>
+  </si>
+  <si>
+    <t>waap</t>
+  </si>
+  <si>
+    <t>ts'ikts'ik</t>
+  </si>
+  <si>
+    <t>x̱aldaawx̱k</t>
+  </si>
+  <si>
+    <t>an'on</t>
+  </si>
+  <si>
+    <t>naks</t>
+  </si>
+  <si>
+    <t>kap</t>
+  </si>
+  <si>
+    <t>g̱oot</t>
+  </si>
+  <si>
+    <t>wüliilm tgwah</t>
+  </si>
+  <si>
+    <t>g̱aayt</t>
+  </si>
+  <si>
+    <t>hooya</t>
+  </si>
+  <si>
+    <t>g̱aws</t>
+  </si>
+  <si>
+    <t>ha'ligyet</t>
+  </si>
+  <si>
+    <t>grandfather</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>father</t>
+  </si>
+  <si>
+    <t>cousin</t>
+  </si>
+  <si>
+    <t>a woman's brother</t>
+  </si>
+  <si>
+    <t>a man's brother</t>
+  </si>
+  <si>
+    <t>child (of someone)</t>
+  </si>
+  <si>
+    <t>coat</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>house</t>
+  </si>
+  <si>
+    <t>dollar; money</t>
+  </si>
+  <si>
+    <t>medicine</t>
+  </si>
+  <si>
+    <t>hand or arm</t>
+  </si>
+  <si>
+    <t>spouse</t>
+  </si>
+  <si>
+    <t>cup</t>
+  </si>
+  <si>
+    <t>heart/mind</t>
+  </si>
+  <si>
+    <t>glasses</t>
+  </si>
+  <si>
+    <t>hat</t>
+  </si>
+  <si>
+    <t>clothes</t>
+  </si>
+  <si>
+    <t>hair</t>
+  </si>
+  <si>
+    <t>birthday</t>
   </si>
 </sst>
 </file>
@@ -477,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC874A0-24D6-4D58-943B-C8A3DC2DA381}">
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,6 +668,9 @@
       <c r="E2" t="s">
         <v>14</v>
       </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -546,10 +678,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -557,14 +689,14 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>1+A3</f>
+        <f t="shared" ref="A4:A67" si="0">1+A3</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -572,8 +704,17 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" ref="A5:A68" si="0">1+A4</f>
+        <f t="shared" si="0"/>
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -581,158 +722,341 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -950,13 +1274,13 @@
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A68:A85" si="1">1+A67</f>
         <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69">
-        <f t="shared" ref="A69:A87" si="1">1+A68</f>
+        <f t="shared" si="1"/>
         <v>68</v>
       </c>
     </row>
@@ -1054,18 +1378,6 @@
       <c r="A85">
         <f t="shared" si="1"/>
         <v>84</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86">
-        <f t="shared" si="1"/>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87">
-        <f t="shared" si="1"/>
-        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update fst, lexc, and JSONs
</commit_message>
<xml_diff>
--- a/fst/dict_sgx.xlsx
+++ b/fst/dict_sgx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d59e73f3ee902bc/Desktop/repos/sguuxs_splicer/fst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DD866BF-63A4-4FDD-BFDF-64B9B761C821}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D41D9D6-9972-494D-8BD5-8E3B6EA16B81}"/>
   <bookViews>
-    <workbookView xWindow="4992" yWindow="504" windowWidth="17280" windowHeight="10560" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
   <si>
     <t>Entry ID</t>
   </si>
@@ -222,6 +222,33 @@
   </si>
   <si>
     <t>birthday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ał </t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>preposition</t>
+  </si>
+  <si>
+    <t>łaxi</t>
+  </si>
+  <si>
+    <t>under</t>
+  </si>
+  <si>
+    <t>lax̱'oi</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>ts'm</t>
+  </si>
+  <si>
+    <t>in</t>
   </si>
 </sst>
 </file>
@@ -263,9 +290,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -608,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC874A0-24D6-4D58-943B-C8A3DC2DA381}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1025,23 +1055,59 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
+      <c r="B26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated csv & rules
</commit_message>
<xml_diff>
--- a/fst/dict_sgx.xlsx
+++ b/fst/dict_sgx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d59e73f3ee902bc/Desktop/repos/sguuxs_splicer/fst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D41D9D6-9972-494D-8BD5-8E3B6EA16B81}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D902B512-A110-4F4F-B7F6-7E2D4551125E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
   <si>
     <t>Entry ID</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>in</t>
+  </si>
+  <si>
+    <t>ei</t>
   </si>
 </sst>
 </file>
@@ -639,7 +642,7 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,7 +918,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -930,7 +933,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -945,7 +948,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -960,7 +963,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -975,7 +978,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -990,7 +993,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1005,7 +1008,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1020,7 +1023,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1035,7 +1038,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1050,7 +1053,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1064,8 +1067,11 @@
       <c r="E26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="I26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1080,7 +1086,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1095,7 +1101,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1110,19 +1116,19 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>

</xml_diff>

<commit_message>
sgx_full & json changes
</commit_message>
<xml_diff>
--- a/fst/dict_sgx.xlsx
+++ b/fst/dict_sgx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d59e73f3ee902bc/Desktop/repos/sguuxs_splicer/fst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{855B4B3E-84BB-4079-8A10-34A9F45871BA}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85E15470-971D-49C5-99DB-C0CF3934EF35}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="1320" windowWidth="17280" windowHeight="8880" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -239,9 +239,6 @@
     <t>lax̱'oi</t>
   </si>
   <si>
-    <t>on</t>
-  </si>
-  <si>
     <t>ts'm</t>
   </si>
   <si>
@@ -252,6 +249,9 @@
   </si>
   <si>
     <t>łguułk</t>
+  </si>
+  <si>
+    <t>on (top)</t>
   </si>
 </sst>
 </file>
@@ -316,6 +316,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -637,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC874A0-24D6-4D58-943B-C8A3DC2DA381}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,7 +804,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>46</v>
@@ -1073,7 +1077,7 @@
         <v>63</v>
       </c>
       <c r="I26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1100,7 +1104,7 @@
         <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E28" t="s">
         <v>63</v>
@@ -1112,10 +1116,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
         <v>68</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
       </c>
       <c r="E29" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
updated messy words rules
</commit_message>
<xml_diff>
--- a/fst/dict_sgx.xlsx
+++ b/fst/dict_sgx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d59e73f3ee902bc/Desktop/repos/sguuxs_splicer/fst/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d59e73f3ee902bc/Desktop/sguuxs_splicer/fst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C50C08AC-EE35-4ABE-833F-C0D3AAD11A23}"/>
+  <xr:revisionPtr revIDLastSave="241" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7DC2E30-A913-4939-B4FB-4844ED984F02}"/>
   <bookViews>
-    <workbookView xWindow="5232" yWindow="1032" windowWidth="17280" windowHeight="10968" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -209,9 +209,6 @@
     <t>at</t>
   </si>
   <si>
-    <t>preposition</t>
-  </si>
-  <si>
     <t>łaxi</t>
   </si>
   <si>
@@ -462,6 +459,9 @@
   </si>
   <si>
     <t>All counting</t>
+  </si>
+  <si>
+    <t>prenoun</t>
   </si>
 </sst>
 </file>
@@ -527,10 +527,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -852,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC874A0-24D6-4D58-943B-C8A3DC2DA381}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K76" sqref="K76"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,7 +951,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -1000,7 +996,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -1015,7 +1011,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
         <v>40</v>
@@ -1129,7 +1125,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
         <v>45</v>
@@ -1189,7 +1185,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
         <v>49</v>
@@ -1219,7 +1215,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
         <v>51</v>
@@ -1249,7 +1245,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
         <v>53</v>
@@ -1285,10 +1281,10 @@
         <v>56</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>141</v>
       </c>
       <c r="I26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1297,13 +1293,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
         <v>58</v>
       </c>
-      <c r="C27" t="s">
-        <v>59</v>
-      </c>
       <c r="E27" t="s">
-        <v>57</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1312,13 +1308,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1327,13 +1323,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
         <v>60</v>
       </c>
-      <c r="C29" t="s">
-        <v>61</v>
-      </c>
       <c r="E29" t="s">
-        <v>57</v>
+        <v>141</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1345,16 +1341,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" t="s">
         <v>73</v>
       </c>
-      <c r="C30" t="s">
-        <v>74</v>
-      </c>
       <c r="E30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1363,16 +1359,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1381,16 +1377,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1399,16 +1395,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -1417,16 +1413,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1435,16 +1431,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -1453,16 +1449,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" t="s">
         <v>85</v>
       </c>
-      <c r="C36" t="s">
-        <v>86</v>
-      </c>
       <c r="E36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1471,16 +1467,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" t="s">
         <v>87</v>
       </c>
-      <c r="C37" t="s">
-        <v>88</v>
-      </c>
       <c r="E37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -1489,16 +1485,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -1507,16 +1503,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -1525,16 +1521,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -1543,16 +1539,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -1561,16 +1557,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -1579,16 +1575,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -1597,16 +1593,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -1615,16 +1611,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -1633,16 +1629,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -1651,16 +1647,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
@@ -1669,16 +1665,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
@@ -1687,19 +1683,19 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49" t="s">
+        <v>71</v>
+      </c>
+      <c r="I49" t="s">
         <v>103</v>
       </c>
-      <c r="C49" t="s">
-        <v>83</v>
-      </c>
-      <c r="E49" t="s">
-        <v>72</v>
-      </c>
-      <c r="I49" t="s">
-        <v>104</v>
-      </c>
       <c r="K49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
@@ -1708,16 +1704,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
@@ -1726,16 +1722,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C51" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
@@ -1744,19 +1740,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" t="s">
+        <v>87</v>
+      </c>
+      <c r="E52" t="s">
+        <v>71</v>
+      </c>
+      <c r="I52" t="s">
         <v>107</v>
       </c>
-      <c r="C52" t="s">
-        <v>88</v>
-      </c>
-      <c r="E52" t="s">
-        <v>72</v>
-      </c>
-      <c r="I52" t="s">
-        <v>108</v>
-      </c>
       <c r="K52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
@@ -1765,16 +1761,16 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
@@ -1783,16 +1779,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E54" t="s">
+        <v>71</v>
+      </c>
+      <c r="K54" t="s">
         <v>110</v>
-      </c>
-      <c r="C54" t="s">
-        <v>92</v>
-      </c>
-      <c r="E54" t="s">
-        <v>72</v>
-      </c>
-      <c r="K54" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
@@ -1801,16 +1797,16 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E55" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
@@ -1819,16 +1815,16 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
@@ -1837,16 +1833,16 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
@@ -1855,16 +1851,16 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
@@ -1873,16 +1869,16 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K59" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
@@ -1891,16 +1887,16 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
@@ -1909,16 +1905,16 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K61" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
@@ -1927,19 +1923,19 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" t="s">
+        <v>87</v>
+      </c>
+      <c r="E62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I62" t="s">
         <v>120</v>
       </c>
-      <c r="C62" t="s">
-        <v>88</v>
-      </c>
-      <c r="E62" t="s">
-        <v>72</v>
-      </c>
-      <c r="I62" t="s">
-        <v>121</v>
-      </c>
       <c r="K62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
@@ -1948,16 +1944,16 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K63" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
@@ -1966,16 +1962,16 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" t="s">
+        <v>91</v>
+      </c>
+      <c r="E64" t="s">
+        <v>71</v>
+      </c>
+      <c r="K64" t="s">
         <v>123</v>
-      </c>
-      <c r="C64" t="s">
-        <v>92</v>
-      </c>
-      <c r="E64" t="s">
-        <v>72</v>
-      </c>
-      <c r="K64" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
@@ -1984,16 +1980,16 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
@@ -2002,16 +1998,16 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C66" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
@@ -2020,16 +2016,16 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C67" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E67" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
@@ -2038,16 +2034,16 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
@@ -2056,16 +2052,16 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K69" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
@@ -2074,19 +2070,19 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>129</v>
+      </c>
+      <c r="C70" t="s">
+        <v>83</v>
+      </c>
+      <c r="E70" t="s">
+        <v>71</v>
+      </c>
+      <c r="I70" t="s">
         <v>130</v>
       </c>
-      <c r="C70" t="s">
-        <v>84</v>
-      </c>
-      <c r="E70" t="s">
-        <v>72</v>
-      </c>
-      <c r="I70" t="s">
-        <v>131</v>
-      </c>
       <c r="K70" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
@@ -2095,16 +2091,16 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K71" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
@@ -2113,19 +2109,19 @@
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C72" t="s">
+        <v>87</v>
+      </c>
+      <c r="E72" t="s">
+        <v>71</v>
+      </c>
+      <c r="I72" t="s">
         <v>133</v>
       </c>
-      <c r="C72" t="s">
-        <v>88</v>
-      </c>
-      <c r="E72" t="s">
-        <v>72</v>
-      </c>
-      <c r="I72" t="s">
-        <v>134</v>
-      </c>
       <c r="K72" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
@@ -2134,16 +2130,16 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K73" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
@@ -2152,19 +2148,19 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74" t="s">
+        <v>91</v>
+      </c>
+      <c r="E74" t="s">
+        <v>71</v>
+      </c>
+      <c r="I74" t="s">
         <v>136</v>
       </c>
-      <c r="C74" t="s">
-        <v>92</v>
-      </c>
-      <c r="E74" t="s">
-        <v>72</v>
-      </c>
-      <c r="I74" t="s">
+      <c r="K74" t="s">
         <v>137</v>
-      </c>
-      <c r="K74" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
@@ -2173,16 +2169,16 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
+        <v>138</v>
+      </c>
+      <c r="C75" t="s">
         <v>139</v>
       </c>
-      <c r="C75" t="s">
+      <c r="E75" t="s">
+        <v>71</v>
+      </c>
+      <c r="K75" t="s">
         <v>140</v>
-      </c>
-      <c r="E75" t="s">
-        <v>72</v>
-      </c>
-      <c r="K75" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated rules, spacing and { }
</commit_message>
<xml_diff>
--- a/fst/dict_sgx.xlsx
+++ b/fst/dict_sgx.xlsx
@@ -852,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC874A0-24D6-4D58-943B-C8A3DC2DA381}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated rules/csv with lexicon
</commit_message>
<xml_diff>
--- a/fst/dict_sgx.xlsx
+++ b/fst/dict_sgx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d59e73f3ee902bc/Desktop/repos/sguuxs_splicer/fst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="283" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F254FE45-FF7D-46BE-A3BD-B44EF052EB96}"/>
+  <xr:revisionPtr revIDLastSave="316" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90AA9B8A-9683-4E69-BB37-DBAC074AD693}"/>
   <bookViews>
-    <workbookView xWindow="1188" yWindow="960" windowWidth="21132" windowHeight="8880" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="151">
   <si>
     <t>Entry ID</t>
   </si>
@@ -462,6 +462,33 @@
   </si>
   <si>
     <t>łax</t>
+  </si>
+  <si>
+    <t>noo</t>
+  </si>
+  <si>
+    <t>mom</t>
+  </si>
+  <si>
+    <t>noho</t>
+  </si>
+  <si>
+    <t>łmkdii</t>
+  </si>
+  <si>
+    <t>sibling (either gender)</t>
+  </si>
+  <si>
+    <t>'yaxwt</t>
+  </si>
+  <si>
+    <t>man</t>
+  </si>
+  <si>
+    <t>hoon</t>
+  </si>
+  <si>
+    <t>fish</t>
   </si>
 </sst>
 </file>
@@ -503,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -512,6 +539,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC874A0-24D6-4D58-943B-C8A3DC2DA381}">
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I83" sqref="I83"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2052,7 +2080,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
-        <f t="shared" ref="A69:A87" si="1">1+A68</f>
+        <f t="shared" ref="A69:A92" si="1">1+A68</f>
         <v>68</v>
       </c>
       <c r="B69" t="s">
@@ -2211,8 +2239,8 @@
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>12</v>
+      <c r="B77" t="s">
+        <v>16</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>13</v>
@@ -2223,8 +2251,9 @@
       <c r="G77">
         <v>1</v>
       </c>
-      <c r="I77" t="s">
-        <v>16</v>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
@@ -2355,23 +2384,104 @@
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
+      <c r="B84" t="s">
+        <v>142</v>
+      </c>
+      <c r="C84" t="s">
+        <v>143</v>
+      </c>
+      <c r="E84" t="s">
+        <v>14</v>
+      </c>
+      <c r="I84" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
+      <c r="B85" t="s">
+        <v>144</v>
+      </c>
+      <c r="C85" t="s">
+        <v>143</v>
+      </c>
+      <c r="E85" t="s">
+        <v>14</v>
+      </c>
+      <c r="I85" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
+      <c r="B86" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C86" t="s">
+        <v>146</v>
+      </c>
+      <c r="E86" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87">
+        <f>1+A86</f>
+        <v>86</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C87" t="s">
+        <v>148</v>
+      </c>
+      <c r="E87" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A88">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>149</v>
+      </c>
+      <c r="C88" t="s">
+        <v>150</v>
+      </c>
+      <c r="E88" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <f t="shared" si="1"/>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
regex for stems added
</commit_message>
<xml_diff>
--- a/fst/dict_sgx.xlsx
+++ b/fst/dict_sgx.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="316" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90AA9B8A-9683-4E69-BB37-DBAC074AD693}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
+    <workbookView xWindow="-23625" yWindow="1695" windowWidth="17280" windowHeight="8880" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -880,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC874A0-24D6-4D58-943B-C8A3DC2DA381}">
   <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H81" sqref="H81"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated suffix test and corresponding vocab
</commit_message>
<xml_diff>
--- a/fst/dict_sgx.xlsx
+++ b/fst/dict_sgx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d59e73f3ee902bc/Desktop/repos/sguuxs_splicer/fst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="316" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90AA9B8A-9683-4E69-BB37-DBAC074AD693}"/>
+  <xr:revisionPtr revIDLastSave="331" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{549F2BC1-5560-4C80-B864-212D90242423}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="157">
   <si>
     <t>Entry ID</t>
   </si>
@@ -489,6 +489,24 @@
   </si>
   <si>
     <t>fish</t>
+  </si>
+  <si>
+    <t>chayp</t>
+  </si>
+  <si>
+    <t>bone</t>
+  </si>
+  <si>
+    <t>ba_xbog_mgyemk</t>
+  </si>
+  <si>
+    <t>butterfly</t>
+  </si>
+  <si>
+    <t>wa_t'ukw</t>
+  </si>
+  <si>
+    <t>lingcod</t>
   </si>
 </sst>
 </file>
@@ -880,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC874A0-24D6-4D58-943B-C8A3DC2DA381}">
   <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2465,18 +2483,54 @@
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
+      <c r="B89" t="s">
+        <v>151</v>
+      </c>
+      <c r="C89" t="s">
+        <v>152</v>
+      </c>
+      <c r="E89" t="s">
+        <v>14</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
+      <c r="B90" t="s">
+        <v>153</v>
+      </c>
+      <c r="C90" t="s">
+        <v>154</v>
+      </c>
+      <c r="E90" t="s">
+        <v>14</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
+      </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
+      <c r="B91" t="s">
+        <v>155</v>
+      </c>
+      <c r="C91" t="s">
+        <v>156</v>
+      </c>
+      <c r="E91" t="s">
+        <v>14</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92">

</xml_diff>

<commit_message>
Check rules & test updates
</commit_message>
<xml_diff>
--- a/fst/dict_sgx.xlsx
+++ b/fst/dict_sgx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d59e73f3ee902bc/Desktop/repos/sguuxs_splicer/fst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="331" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{549F2BC1-5560-4C80-B864-212D90242423}"/>
+  <xr:revisionPtr revIDLastSave="356" documentId="8_{E0BE1F1A-7748-469D-BA43-93DDD994B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3488D81F-739F-4744-A4AB-753A3FA0F955}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{6BE07859-709D-48CC-89BD-3E6755E7C80E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="167">
   <si>
     <t>Entry ID</t>
   </si>
@@ -507,6 +507,36 @@
   </si>
   <si>
     <t>lingcod</t>
+  </si>
+  <si>
+    <t>aytk</t>
+  </si>
+  <si>
+    <t>name, identity</t>
+  </si>
+  <si>
+    <t>waan</t>
+  </si>
+  <si>
+    <t>teeth</t>
+  </si>
+  <si>
+    <t>nabiip</t>
+  </si>
+  <si>
+    <t>uncle</t>
+  </si>
+  <si>
+    <t>nikdaa</t>
+  </si>
+  <si>
+    <t>aunt</t>
+  </si>
+  <si>
+    <t>algyax_</t>
+  </si>
+  <si>
+    <t>language, words, speech</t>
   </si>
 </sst>
 </file>
@@ -548,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -557,7 +587,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -896,10 +934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC874A0-24D6-4D58-943B-C8A3DC2DA381}">
-  <dimension ref="A1:L92"/>
+  <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G90" sqref="G90"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -949,7 +987,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -970,7 +1008,7 @@
         <f>1+A2</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C3" t="s">
@@ -985,7 +1023,7 @@
         <f t="shared" ref="A4:A68" si="0">1+A3</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
@@ -1000,7 +1038,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C5" t="s">
@@ -1015,7 +1053,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C6" t="s">
@@ -1030,7 +1068,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
@@ -1045,7 +1083,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C8" t="s">
@@ -1060,7 +1098,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C9" t="s">
@@ -1078,7 +1116,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C10" t="s">
@@ -1093,7 +1131,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C11" t="s">
@@ -1108,7 +1146,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C12" t="s">
@@ -1123,7 +1161,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C13" t="s">
@@ -1138,7 +1176,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C14" t="s">
@@ -1159,7 +1197,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C15" t="s">
@@ -1174,7 +1212,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C16" t="s">
@@ -1189,7 +1227,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C17" t="s">
@@ -1204,7 +1242,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C18" t="s">
@@ -1219,7 +1257,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C19" t="s">
@@ -1234,7 +1272,7 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C20" t="s">
@@ -1249,7 +1287,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C21" t="s">
@@ -1264,7 +1302,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C22" t="s">
@@ -1279,7 +1317,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C23" t="s">
@@ -1294,7 +1332,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C24" t="s">
@@ -1309,7 +1347,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C25" t="s">
@@ -1324,7 +1362,7 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C26" t="s">
@@ -1342,7 +1380,7 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
         <v>141</v>
       </c>
       <c r="C27" t="s">
@@ -1357,7 +1395,7 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="5" t="s">
         <v>139</v>
       </c>
       <c r="C28" t="s">
@@ -1372,7 +1410,7 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C29" t="s">
@@ -1390,7 +1428,7 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C30" t="s">
@@ -1408,7 +1446,7 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C31" t="s">
@@ -1426,7 +1464,7 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
         <v>72</v>
       </c>
       <c r="C32" t="s">
@@ -1444,7 +1482,7 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C33" t="s">
@@ -1462,7 +1500,7 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C34" t="s">
@@ -1480,7 +1518,7 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="5" t="s">
         <v>78</v>
       </c>
       <c r="C35" t="s">
@@ -1498,7 +1536,7 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="5" t="s">
         <v>81</v>
       </c>
       <c r="C36" t="s">
@@ -1516,7 +1554,7 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="5" t="s">
         <v>83</v>
       </c>
       <c r="C37" t="s">
@@ -1534,7 +1572,7 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="5" t="s">
         <v>85</v>
       </c>
       <c r="C38" t="s">
@@ -1552,7 +1590,7 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="5" t="s">
         <v>86</v>
       </c>
       <c r="C39" t="s">
@@ -1570,7 +1608,7 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="5" t="s">
         <v>89</v>
       </c>
       <c r="C40" t="s">
@@ -1588,7 +1626,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C41" t="s">
@@ -1606,7 +1644,7 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C42" t="s">
@@ -1624,7 +1662,7 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="5" t="s">
         <v>92</v>
       </c>
       <c r="C43" t="s">
@@ -1642,7 +1680,7 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="5" t="s">
         <v>93</v>
       </c>
       <c r="C44" t="s">
@@ -1660,7 +1698,7 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="5" t="s">
         <v>108</v>
       </c>
       <c r="C45" t="s">
@@ -1678,7 +1716,7 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="5" t="s">
         <v>96</v>
       </c>
       <c r="C46" t="s">
@@ -1696,7 +1734,7 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="5" t="s">
         <v>97</v>
       </c>
       <c r="C47" t="s">
@@ -1714,7 +1752,7 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="5" t="s">
         <v>98</v>
       </c>
       <c r="C48" t="s">
@@ -1732,7 +1770,7 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="5" t="s">
         <v>99</v>
       </c>
       <c r="C49" t="s">
@@ -1753,7 +1791,7 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="5" t="s">
         <v>101</v>
       </c>
       <c r="C50" t="s">
@@ -1771,7 +1809,7 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="5" t="s">
         <v>102</v>
       </c>
       <c r="C51" t="s">
@@ -1789,7 +1827,7 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C52" t="s">
@@ -1810,7 +1848,7 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C53" t="s">
@@ -1828,7 +1866,7 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="5" t="s">
         <v>106</v>
       </c>
       <c r="C54" t="s">
@@ -1846,7 +1884,7 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C55" t="s">
@@ -1864,7 +1902,7 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="5" t="s">
         <v>110</v>
       </c>
       <c r="C56" t="s">
@@ -1882,7 +1920,7 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="5" t="s">
         <v>111</v>
       </c>
       <c r="C57" t="s">
@@ -1900,7 +1938,7 @@
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C58" t="s">
@@ -1918,7 +1956,7 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="5" t="s">
         <v>113</v>
       </c>
       <c r="C59" t="s">
@@ -1936,7 +1974,7 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C60" t="s">
@@ -1954,7 +1992,7 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="5" t="s">
         <v>115</v>
       </c>
       <c r="C61" t="s">
@@ -1972,7 +2010,7 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="5" t="s">
         <v>116</v>
       </c>
       <c r="C62" t="s">
@@ -1993,7 +2031,7 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="5" t="s">
         <v>118</v>
       </c>
       <c r="C63" t="s">
@@ -2011,7 +2049,7 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C64" t="s">
@@ -2029,7 +2067,7 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="5" t="s">
         <v>121</v>
       </c>
       <c r="C65" t="s">
@@ -2047,7 +2085,7 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="5" t="s">
         <v>122</v>
       </c>
       <c r="C66" t="s">
@@ -2065,7 +2103,7 @@
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="5" t="s">
         <v>123</v>
       </c>
       <c r="C67" t="s">
@@ -2083,7 +2121,7 @@
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="5" t="s">
         <v>124</v>
       </c>
       <c r="C68" t="s">
@@ -2098,10 +2136,10 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
-        <f t="shared" ref="A69:A92" si="1">1+A68</f>
-        <v>68</v>
-      </c>
-      <c r="B69" t="s">
+        <f t="shared" ref="A69:A96" si="1">1+A68</f>
+        <v>68</v>
+      </c>
+      <c r="B69" s="5" t="s">
         <v>125</v>
       </c>
       <c r="C69" t="s">
@@ -2119,7 +2157,7 @@
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="5" t="s">
         <v>126</v>
       </c>
       <c r="C70" t="s">
@@ -2140,7 +2178,7 @@
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="5" t="s">
         <v>128</v>
       </c>
       <c r="C71" t="s">
@@ -2158,7 +2196,7 @@
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C72" t="s">
@@ -2179,7 +2217,7 @@
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="5" t="s">
         <v>131</v>
       </c>
       <c r="C73" t="s">
@@ -2197,7 +2235,7 @@
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="5" t="s">
         <v>132</v>
       </c>
       <c r="C74" t="s">
@@ -2218,7 +2256,7 @@
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="5" t="s">
         <v>135</v>
       </c>
       <c r="C75" t="s">
@@ -2236,7 +2274,7 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C76" t="s">
@@ -2257,7 +2295,7 @@
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C77" s="1" t="s">
@@ -2279,7 +2317,7 @@
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="5" t="s">
         <v>127</v>
       </c>
       <c r="C78" t="s">
@@ -2300,7 +2338,7 @@
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C79" t="s">
@@ -2321,7 +2359,7 @@
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="5" t="s">
         <v>104</v>
       </c>
       <c r="C80" t="s">
@@ -2342,7 +2380,7 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="5" t="s">
         <v>130</v>
       </c>
       <c r="C81" t="s">
@@ -2363,7 +2401,7 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="5" t="s">
         <v>133</v>
       </c>
       <c r="C82" t="s">
@@ -2384,7 +2422,7 @@
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="6" t="s">
         <v>60</v>
       </c>
       <c r="C83" t="s">
@@ -2402,7 +2440,7 @@
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="5" t="s">
         <v>142</v>
       </c>
       <c r="C84" t="s">
@@ -2420,7 +2458,7 @@
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="5" t="s">
         <v>144</v>
       </c>
       <c r="C85" t="s">
@@ -2438,7 +2476,7 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="8" t="s">
         <v>145</v>
       </c>
       <c r="C86" t="s">
@@ -2453,7 +2491,7 @@
         <f>1+A86</f>
         <v>86</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="8" t="s">
         <v>147</v>
       </c>
       <c r="C87" t="s">
@@ -2468,7 +2506,7 @@
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="5" t="s">
         <v>149</v>
       </c>
       <c r="C88" t="s">
@@ -2483,7 +2521,7 @@
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="5" t="s">
         <v>151</v>
       </c>
       <c r="C89" t="s">
@@ -2501,7 +2539,7 @@
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="5" t="s">
         <v>153</v>
       </c>
       <c r="C90" t="s">
@@ -2519,7 +2557,7 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="5" t="s">
         <v>155</v>
       </c>
       <c r="C91" t="s">
@@ -2537,6 +2575,90 @@
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
+      <c r="B92" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C92" t="s">
+        <v>158</v>
+      </c>
+      <c r="E92" t="s">
+        <v>14</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C93" t="s">
+        <v>160</v>
+      </c>
+      <c r="E93" t="s">
+        <v>14</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C94" t="s">
+        <v>162</v>
+      </c>
+      <c r="E94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C95" t="s">
+        <v>164</v>
+      </c>
+      <c r="E95" t="s">
+        <v>14</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C96" t="s">
+        <v>166</v>
+      </c>
+      <c r="E96" t="s">
+        <v>14</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>